<commit_message>
Refactor User Authentication and Password Comparison Enhancements
- Improved password comparison logic in UserRepository to handle various numeric formats and scenarios.
- Updated AccountController's LoginDebug endpoint for clearer routing and enhanced descriptions, removing unnecessary development restrictions.
</commit_message>
<xml_diff>
--- a/CNCToolingDatabase/Data/USER MASTER.xlsx
+++ b/CNCToolingDatabase/Data/USER MASTER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Tool-Master-Control\Tool-Master-Control\CNCToolingDatabase\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EF5F8A-89FC-4C9D-BFCD-81138CED18B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030FEE93-8B91-470F-A6B2-B5357DA84D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8271D9D6-2065-419F-AC52-7850B71D4074}"/>
+    <workbookView xWindow="1455" yWindow="3570" windowWidth="21600" windowHeight="11295" xr2:uid="{8271D9D6-2065-419F-AC52-7850B71D4074}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>No.</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>abc123</t>
   </si>
 </sst>
 </file>
@@ -185,10 +188,6 @@
   <dxfs count="7">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -205,6 +204,10 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -287,9 +290,9 @@
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{4A87BED8-B1B5-45DE-BB4C-8C3E6116591E}" name="No." dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{5E55A1C0-5160-4819-9AC4-BFE97197F01A}" name="Username" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{9E99972C-6257-4496-92A9-7B0B9EFC93FF}" name="Password" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{E05168FF-5C3E-4D5A-B93D-D4D10BF8E5D9}" name="Display Name" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{F3A2A34E-F6A4-4E74-965D-DE476ADF2610}" name="Status" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{9E99972C-6257-4496-92A9-7B0B9EFC93FF}" name="Password" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{E05168FF-5C3E-4D5A-B93D-D4D10BF8E5D9}" name="Display Name" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{F3A2A34E-F6A4-4E74-965D-DE476ADF2610}" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -595,7 +598,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,8 +635,8 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3">
-        <v>123</v>
+      <c r="C2" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>4</v>
@@ -649,8 +652,8 @@
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3">
-        <v>123</v>
+      <c r="C3" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>6</v>
@@ -666,8 +669,8 @@
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3">
-        <v>123</v>
+      <c r="C4" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>8</v>
@@ -683,8 +686,8 @@
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3">
-        <v>123</v>
+      <c r="C5" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>10</v>
@@ -700,8 +703,8 @@
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3">
-        <v>123</v>
+      <c r="C6" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>12</v>
@@ -717,8 +720,8 @@
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="3">
-        <v>123</v>
+      <c r="C7" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>14</v>
@@ -734,8 +737,8 @@
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="3">
-        <v>123</v>
+      <c r="C8" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>16</v>
@@ -751,8 +754,8 @@
       <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="3">
-        <v>123</v>
+      <c r="C9" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>18</v>
@@ -768,8 +771,8 @@
       <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="3">
-        <v>123</v>
+      <c r="C10" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>20</v>
@@ -785,8 +788,8 @@
       <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="3">
-        <v>123</v>
+      <c r="C11" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>23</v>

</xml_diff>